<commit_message>
PROS-6581 - CCRU - new KPI tables and POS 2019
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/KPI_Source.xlsx
+++ b/Projects/CCRU/Data/KPI_Source.xlsx
@@ -236,7 +236,7 @@
     <t xml:space="preserve">KPIs_2019/PoS 2019 - FT - CAP.xlsx</t>
   </si>
   <si>
-    <t xml:space="preserve">KPIs_2019/Gaps Guide 2018.xlsx</t>
+    <t xml:space="preserve">KPIs_2019/Gaps Guide 2019.xlsx</t>
   </si>
   <si>
     <t xml:space="preserve">KPIs_2019/Spirits 2018 - FT.xlsx</t>
@@ -629,10 +629,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.3112244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.7704081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -786,10 +787,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.719387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.1122448979592"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.719387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.3112244897959"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.5714285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.3112244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -937,10 +939,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.719387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.1122448979592"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.719387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.3112244897959"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.5714285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.3112244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1083,16 +1086,16 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.9387755102041"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.530612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1131,7 +1134,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>5</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1210,11 +1213,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.9387755102041"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.530612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1253,7 +1256,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>5</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1332,11 +1335,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.9387755102041"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.530612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1375,7 +1378,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>5</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1454,11 +1457,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.9387755102041"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.530612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1497,7 +1500,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1576,11 +1579,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.4336734693878"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.1734693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.1632653061224"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.6326530612245"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1619,7 +1622,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1722,11 +1725,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.4336734693878"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.1734693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.1632653061224"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.6326530612245"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1765,7 +1768,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>53</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1868,11 +1871,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.1785714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="48.8673469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.6377551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="48.3265306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1911,7 +1914,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>45</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2020,11 +2023,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.1785714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="48.8673469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.6377551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="48.3265306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2063,7 +2066,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>45</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2172,10 +2175,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.3112244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.0255102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.7704081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.75"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2329,11 +2333,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.1785714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="48.8673469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.6377551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="48.3265306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2372,7 +2376,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>51</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2481,11 +2485,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.1785714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="48.8673469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.6377551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="48.3265306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2524,7 +2528,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>51</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2633,10 +2637,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.719387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.1122448979592"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.719387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.3112244897959"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.5714285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.3112244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2675,7 +2680,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>55</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2778,10 +2783,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.719387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.1122448979592"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.719387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.3112244897959"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.5714285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.3112244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2820,7 +2826,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>55</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2923,10 +2929,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.719387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.1122448979592"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.719387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.3112244897959"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.5714285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.3112244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2965,7 +2972,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>57</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3068,10 +3075,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.0663265306122"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.5255102040816"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.75"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3110,7 +3118,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>39</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3219,10 +3227,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.0663265306122"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.5255102040816"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.75"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3261,7 +3270,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>39</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3370,10 +3379,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.9591836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.5510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.75"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3412,7 +3422,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>39</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3521,10 +3531,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.9591836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.5510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.75"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3563,7 +3574,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>39</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3672,10 +3683,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.3112244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.0255102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.7704081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.75"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3714,7 +3726,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>31</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3823,10 +3835,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.3112244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.0255102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.7704081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.75"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3980,10 +3993,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.3112244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.0255102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.7704081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.75"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4022,7 +4036,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>31</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4131,10 +4145,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.3061224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.0255102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.765306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.75"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4173,7 +4188,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>35</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4277,15 +4292,16 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="N32" activeCellId="0" sqref="N32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.8469387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.0255102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.3061224489796"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.75"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4324,7 +4340,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>35</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4433,10 +4449,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.3112244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.7704081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.75"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4590,10 +4607,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.3112244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.0255102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.7704081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.75"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4747,10 +4765,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.719387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.1122448979592"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.719387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.3112244897959"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.5714285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.3112244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4904,10 +4923,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.719387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.1122448979592"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.719387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.3112244897959"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.5714285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.3112244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5061,10 +5081,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.719387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.1122448979592"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.719387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.3112244897959"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.5714285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.3112244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5218,10 +5239,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.719387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.1122448979592"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.719387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.3112244897959"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.5714285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.3112244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
PROS-8387 - CCRU - Calculate Benchmark - Development
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/KPI_Source.xlsx
+++ b/Projects/CCRU/Data/KPI_Source.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="11" activeTab="20"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="11" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Pos 2018 - FT" sheetId="1" state="hidden" r:id="rId2"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1106" uniqueCount="139">
   <si>
     <t xml:space="preserve">SOURCE</t>
   </si>
@@ -242,6 +242,18 @@
     <t xml:space="preserve">KPIs_2019/Spirits 2018 - FT.xlsx</t>
   </si>
   <si>
+    <t xml:space="preserve">BENCHMARK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benchmark</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPIs_2019/Benchmark 2019.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FT</t>
+  </si>
+  <si>
     <t xml:space="preserve">PoS 2019 - FT - REG</t>
   </si>
   <si>
@@ -254,12 +266,18 @@
     <t xml:space="preserve">KPIs_2019/PoS 2019 - FT NS - CAP.xlsx</t>
   </si>
   <si>
+    <t xml:space="preserve">FT NS CAP</t>
+  </si>
+  <si>
     <t xml:space="preserve">PoS 2019 - FT NS - REG</t>
   </si>
   <si>
     <t xml:space="preserve">KPIs_2019/PoS 2019 - FT NS - REG.xlsx</t>
   </si>
   <si>
+    <t xml:space="preserve">FT NS REG</t>
+  </si>
+  <si>
     <t xml:space="preserve">PoS 2019 - IC Canteen - EDU</t>
   </si>
   <si>
@@ -287,12 +305,18 @@
     <t xml:space="preserve">KPIs_2019/KPIConversion2019.xlsx</t>
   </si>
   <si>
+    <t xml:space="preserve">Canteen EDU</t>
+  </si>
+  <si>
     <t xml:space="preserve">PoS 2019 - IC Canteen - OTH</t>
   </si>
   <si>
     <t xml:space="preserve">KPIs_2019/PoS 2019 - IC Canteen - OTH.xlsx</t>
   </si>
   <si>
+    <t xml:space="preserve">Canteen OTH</t>
+  </si>
+  <si>
     <t xml:space="preserve">PoS 2019 - IC HoReCa BarTavernClub - CAP</t>
   </si>
   <si>
@@ -308,6 +332,9 @@
     <t xml:space="preserve">IC - HoReCa All</t>
   </si>
   <si>
+    <t xml:space="preserve">HoReCa</t>
+  </si>
+  <si>
     <t xml:space="preserve">PoS 2019 - IC HoReCa BarTavernClub - REG</t>
   </si>
   <si>
@@ -344,6 +371,9 @@
     <t xml:space="preserve">IC - Petroleum</t>
   </si>
   <si>
+    <t xml:space="preserve">Petrol</t>
+  </si>
+  <si>
     <t xml:space="preserve">PoS 2019 - IC Petroleum - REG</t>
   </si>
   <si>
@@ -359,6 +389,9 @@
     <t xml:space="preserve">IC - QSR</t>
   </si>
   <si>
+    <t xml:space="preserve">QSR</t>
+  </si>
+  <si>
     <t xml:space="preserve">PoS 2019 - MT Conv Big - CAP</t>
   </si>
   <si>
@@ -371,12 +404,18 @@
     <t xml:space="preserve">MT - Conv All</t>
   </si>
   <si>
+    <t xml:space="preserve">Conv Big CAP</t>
+  </si>
+  <si>
     <t xml:space="preserve">PoS 2019 - MT Conv Big - REG</t>
   </si>
   <si>
     <t xml:space="preserve">KPIs_2019/PoS 2019 - MT Conv Big - REG.xlsx</t>
   </si>
   <si>
+    <t xml:space="preserve">Conv Other</t>
+  </si>
+  <si>
     <t xml:space="preserve">PoS 2019 - MT Conv Small - CAP</t>
   </si>
   <si>
@@ -401,6 +440,9 @@
     <t xml:space="preserve">MT - Hyper-Super</t>
   </si>
   <si>
+    <t xml:space="preserve">Hyper</t>
+  </si>
+  <si>
     <t xml:space="preserve">PoS 2019 - MT Hypermarket - REG</t>
   </si>
   <si>
@@ -416,10 +458,16 @@
     <t xml:space="preserve">KPIs_2019/Spirits 2018 - MT - Supermarket.xlsx</t>
   </si>
   <si>
+    <t xml:space="preserve">Super CAP</t>
+  </si>
+  <si>
     <t xml:space="preserve">PoS 2019 - MT Supermarket - REG</t>
   </si>
   <si>
     <t xml:space="preserve">KPIs_2019/PoS 2019 - MT Supermarket - REG.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Super REG</t>
   </si>
 </sst>
 </file>
@@ -459,7 +507,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -494,6 +542,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF99FFFF"/>
         <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9900"/>
+        <bgColor rgb="FFFFCC00"/>
       </patternFill>
     </fill>
     <fill>
@@ -537,7 +597,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -563,6 +623,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -651,11 +719,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.234693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.25"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.4234693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.6887755102041"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -809,11 +876,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.7704081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.030612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.7704081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.8265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.8163265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.8265306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -961,11 +1027,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.7704081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.030612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.7704081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.8265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.8163265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.8265306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1105,18 +1170,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.1275510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.3163265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1208,6 +1274,20 @@
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1226,7 +1306,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
@@ -1234,10 +1314,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.1275510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.3163265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1259,10 +1340,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1276,7 +1357,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1329,6 +1410,20 @@
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1347,18 +1442,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.1275510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.3163265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1380,10 +1476,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1397,7 +1493,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1450,6 +1546,20 @@
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1468,18 +1578,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.1275510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.3163265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1501,10 +1612,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1518,7 +1629,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1571,6 +1682,20 @@
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1589,18 +1714,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.0918367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.280612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1622,10 +1748,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1639,7 +1765,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1647,10 +1773,10 @@
         <v>10</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1668,13 +1794,13 @@
         <v>19</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1682,13 +1808,13 @@
         <v>22</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1715,7 +1841,21 @@
         <v>29</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>77</v>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1734,18 +1874,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.0918367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.280612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1767,10 +1908,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1784,7 +1925,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1792,10 +1933,10 @@
         <v>10</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1813,13 +1954,13 @@
         <v>19</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1827,13 +1968,13 @@
         <v>22</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1860,7 +2001,21 @@
         <v>29</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>77</v>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1879,18 +2034,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.0969387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.6530612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.2857142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.5714285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1912,10 +2068,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1928,8 +2084,8 @@
       <c r="C3" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>82</v>
+      <c r="D3" s="8" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1937,10 +2093,10 @@
         <v>10</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1956,7 +2112,7 @@
         <v>47</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1964,13 +2120,13 @@
         <v>19</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1978,13 +2134,13 @@
         <v>22</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2011,7 +2167,21 @@
         <v>29</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>77</v>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -2030,7 +2200,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
@@ -2038,10 +2208,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.0969387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.6530612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.2857142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.5714285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2063,10 +2234,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2079,8 +2250,8 @@
       <c r="C3" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>87</v>
+      <c r="D3" s="8" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2088,10 +2259,10 @@
         <v>10</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2107,7 +2278,7 @@
         <v>47</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2115,13 +2286,13 @@
         <v>19</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2129,13 +2300,13 @@
         <v>22</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2162,7 +2333,21 @@
         <v>29</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>77</v>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -2189,11 +2374,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.6173469387755"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.234693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.3418367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.4234693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.3979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2339,7 +2523,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
@@ -2347,10 +2531,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.0969387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.6530612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.2857142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.5714285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2372,10 +2557,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2388,8 +2573,8 @@
       <c r="C3" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>90</v>
+      <c r="D3" s="8" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2397,10 +2582,10 @@
         <v>10</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2416,7 +2601,7 @@
         <v>47</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2424,13 +2609,13 @@
         <v>19</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2438,13 +2623,13 @@
         <v>22</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2471,7 +2656,21 @@
         <v>29</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>77</v>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -2490,18 +2689,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.0969387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.6530612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.2857142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.5714285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2523,10 +2723,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2539,8 +2739,8 @@
       <c r="C3" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>93</v>
+      <c r="D3" s="8" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2548,10 +2748,10 @@
         <v>10</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2567,7 +2767,7 @@
         <v>47</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2575,13 +2775,13 @@
         <v>19</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2589,13 +2789,13 @@
         <v>22</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2622,7 +2822,21 @@
         <v>29</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>77</v>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -2641,19 +2855,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.7704081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.030612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.7704081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.8265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.8163265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.8265306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2675,10 +2888,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2692,7 +2905,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2700,10 +2913,10 @@
         <v>10</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2721,13 +2934,13 @@
         <v>19</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2735,13 +2948,13 @@
         <v>22</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2768,7 +2981,21 @@
         <v>29</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>77</v>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -2787,7 +3014,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
@@ -2795,11 +3022,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.7704081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.030612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.7704081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.8265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.8163265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.8265306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2821,10 +3047,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2838,7 +3064,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2846,10 +3072,10 @@
         <v>10</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2867,13 +3093,13 @@
         <v>19</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2881,13 +3107,13 @@
         <v>22</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2914,7 +3140,21 @@
         <v>29</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>77</v>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -2933,19 +3173,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.7704081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.030612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.7704081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.8265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.8163265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.8265306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2967,10 +3206,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2984,7 +3223,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2992,10 +3231,10 @@
         <v>10</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3013,13 +3252,13 @@
         <v>19</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3027,13 +3266,13 @@
         <v>22</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3060,7 +3299,21 @@
         <v>29</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>77</v>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -3079,19 +3332,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.1224489795918"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.3418367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.3112244897959"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.3979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3113,10 +3365,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3130,7 +3382,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3138,10 +3390,10 @@
         <v>10</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3157,7 +3409,7 @@
         <v>41</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3165,13 +3417,13 @@
         <v>19</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3179,13 +3431,13 @@
         <v>22</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3212,7 +3464,21 @@
         <v>29</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>77</v>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -3231,19 +3497,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.1224489795918"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.3418367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.3112244897959"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.3979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3265,10 +3530,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3282,7 +3547,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3290,10 +3555,10 @@
         <v>10</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3309,7 +3574,7 @@
         <v>41</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3317,13 +3582,13 @@
         <v>19</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3331,13 +3596,13 @@
         <v>22</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3364,7 +3629,21 @@
         <v>29</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>77</v>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -3383,7 +3662,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
@@ -3391,11 +3670,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.1479591836735"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.3418367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.0663265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.3979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3417,10 +3695,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3434,7 +3712,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3442,10 +3720,10 @@
         <v>10</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3461,7 +3739,7 @@
         <v>41</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3469,13 +3747,13 @@
         <v>19</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3483,13 +3761,13 @@
         <v>22</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3516,7 +3794,21 @@
         <v>29</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>77</v>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -3535,7 +3827,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
@@ -3543,11 +3835,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.1479591836735"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.3418367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.0663265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.3979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3569,10 +3860,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3586,7 +3877,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3594,10 +3885,10 @@
         <v>10</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3613,7 +3904,7 @@
         <v>41</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3621,13 +3912,13 @@
         <v>19</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3635,13 +3926,13 @@
         <v>22</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3668,7 +3959,21 @@
         <v>29</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>77</v>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -3687,19 +3992,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.6173469387755"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.234693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.3418367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.4234693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.3979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3721,10 +4025,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3738,7 +4042,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3746,10 +4050,10 @@
         <v>10</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3765,7 +4069,7 @@
         <v>33</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3773,13 +4077,13 @@
         <v>19</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3787,13 +4091,13 @@
         <v>22</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3820,7 +4124,21 @@
         <v>29</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>77</v>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -3847,11 +4165,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.6173469387755"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.234693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.3418367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.4234693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.3979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3997,7 +4314,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
@@ -4005,11 +4322,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.6173469387755"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.234693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.3418367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.4234693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.3979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4031,10 +4347,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>116</v>
+        <v>130</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>117</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4048,7 +4364,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>116</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4056,10 +4372,10 @@
         <v>10</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4075,7 +4391,7 @@
         <v>33</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4083,13 +4399,13 @@
         <v>19</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4097,13 +4413,13 @@
         <v>22</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4130,7 +4446,21 @@
         <v>29</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>77</v>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -4149,19 +4479,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.6173469387755"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.2295918367347"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.3418367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.4183673469388"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.3979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4183,10 +4512,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>118</v>
+        <v>132</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4200,7 +4529,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>118</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4208,10 +4537,10 @@
         <v>10</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4227,7 +4556,7 @@
         <v>37</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>120</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4235,13 +4564,13 @@
         <v>19</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4249,13 +4578,13 @@
         <v>22</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4282,7 +4611,21 @@
         <v>29</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>77</v>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -4301,19 +4644,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N32" activeCellId="0" sqref="N32"/>
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.6173469387755"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.765306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.3418367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.8214285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.3979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4335,10 +4677,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>122</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4352,7 +4694,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4360,10 +4702,10 @@
         <v>10</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4379,7 +4721,7 @@
         <v>37</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>120</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4387,13 +4729,13 @@
         <v>19</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4401,13 +4743,13 @@
         <v>22</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4434,7 +4776,21 @@
         <v>29</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>77</v>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -4461,11 +4817,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.234693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.3418367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.4234693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.3979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4619,11 +4974,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.6173469387755"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.234693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.3418367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.4234693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.3979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4777,11 +5131,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.7704081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.030612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.7704081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.8265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.8163265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.8265306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4935,11 +5288,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.7704081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.030612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.7704081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.8265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.8163265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.8265306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5093,11 +5445,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.7704081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.030612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.7704081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.8265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.8163265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.8265306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5251,11 +5602,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.7704081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.030612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.7704081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.8265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.8163265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.8265306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
PROS-9738 - CCRU - New POS 2019 KPIs
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/KPI_Source.xlsx
+++ b/Projects/CCRU/Data/KPI_Source.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="11" activeTab="11"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="11" activeTab="27"/>
   </bookViews>
   <sheets>
     <sheet name="Pos 2018 - FT" sheetId="1" state="hidden" r:id="rId2"/>
@@ -25,21 +25,26 @@
     <sheet name="PoS 2019 - FT NS - REG" sheetId="15" state="visible" r:id="rId16"/>
     <sheet name="PoS 2019 - IC Canteen - EDU" sheetId="16" state="visible" r:id="rId17"/>
     <sheet name="PoS 2019 - IC Canteen - OTH" sheetId="17" state="visible" r:id="rId18"/>
-    <sheet name="PoS 2019 - IC HoReCa BarTavernClub - CAP" sheetId="18" state="visible" r:id="rId19"/>
-    <sheet name="PoS 2019 - IC HoReCa BarTavernClub - REG" sheetId="19" state="visible" r:id="rId20"/>
-    <sheet name="PoS 2019 - IC HoReCa RestCafeTea - CAP" sheetId="20" state="visible" r:id="rId21"/>
-    <sheet name="PoS 2019 - IC HoReCa RestCafeTea - REG" sheetId="21" state="visible" r:id="rId22"/>
-    <sheet name="PoS 2019 - IC Petroleum - CAP" sheetId="22" state="visible" r:id="rId23"/>
-    <sheet name="PoS 2019 - IC Petroleum - REG" sheetId="23" state="visible" r:id="rId24"/>
-    <sheet name="PoS 2019 - IC QSR" sheetId="24" state="visible" r:id="rId25"/>
-    <sheet name="PoS 2019 - MT Conv Big - CAP" sheetId="25" state="visible" r:id="rId26"/>
-    <sheet name="PoS 2019 - MT Conv Big - REG" sheetId="26" state="visible" r:id="rId27"/>
-    <sheet name="PoS 2019 - MT Conv Small - CAP" sheetId="27" state="visible" r:id="rId28"/>
-    <sheet name="PoS 2019 - MT Conv Small - REG" sheetId="28" state="visible" r:id="rId29"/>
-    <sheet name="PoS 2019 - MT Hypermarket - CAP" sheetId="29" state="visible" r:id="rId30"/>
-    <sheet name="PoS 2019 - MT Hypermarket - REG" sheetId="30" state="visible" r:id="rId31"/>
-    <sheet name="PoS 2019 - MT Supermarket - CAP" sheetId="31" state="visible" r:id="rId32"/>
-    <sheet name="PoS 2019 - MT Supermarket - REG" sheetId="32" state="visible" r:id="rId33"/>
+    <sheet name="PoS 2019 - IC HoReCa BarTavernClub" sheetId="18" state="visible" r:id="rId19"/>
+    <sheet name="PoS 2019 - IC HoReCa BarTavernClub - CAP" sheetId="19" state="hidden" r:id="rId20"/>
+    <sheet name="PoS 2019 - IC HoReCa BarTavernClub - REG" sheetId="20" state="hidden" r:id="rId21"/>
+    <sheet name="PoS 2019 - IC HoReCa RestCafeTea" sheetId="21" state="visible" r:id="rId22"/>
+    <sheet name="PoS 2019 - IC HoReCa RestCafeTea - CAP" sheetId="22" state="hidden" r:id="rId23"/>
+    <sheet name="PoS 2019 - IC HoReCa RestCafeTea - REG" sheetId="23" state="hidden" r:id="rId24"/>
+    <sheet name="PoS 2019 - IC Petroleum - CAP" sheetId="24" state="visible" r:id="rId25"/>
+    <sheet name="PoS 2019 - IC Petroleum - REG" sheetId="25" state="visible" r:id="rId26"/>
+    <sheet name="PoS 2019 - IC QSR" sheetId="26" state="visible" r:id="rId27"/>
+    <sheet name="PoS 2019 - IC FastFood" sheetId="27" state="visible" r:id="rId28"/>
+    <sheet name="PoS 2019 - IC Cinema - CAP" sheetId="28" state="visible" r:id="rId29"/>
+    <sheet name="PoS 2019 - IC Cinema - REG" sheetId="29" state="visible" r:id="rId30"/>
+    <sheet name="PoS 2019 - MT Conv Big - CAP" sheetId="30" state="visible" r:id="rId31"/>
+    <sheet name="PoS 2019 - MT Conv Big - REG" sheetId="31" state="visible" r:id="rId32"/>
+    <sheet name="PoS 2019 - MT Conv Small - CAP" sheetId="32" state="visible" r:id="rId33"/>
+    <sheet name="PoS 2019 - MT Conv Small - REG" sheetId="33" state="visible" r:id="rId34"/>
+    <sheet name="PoS 2019 - MT Hypermarket - CAP" sheetId="34" state="visible" r:id="rId35"/>
+    <sheet name="PoS 2019 - MT Hypermarket - REG" sheetId="35" state="visible" r:id="rId36"/>
+    <sheet name="PoS 2019 - MT Supermarket - CAP" sheetId="36" state="visible" r:id="rId37"/>
+    <sheet name="PoS 2019 - MT Supermarket - REG" sheetId="37" state="visible" r:id="rId38"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -51,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1106" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1285" uniqueCount="150">
   <si>
     <t xml:space="preserve">SOURCE</t>
   </si>
@@ -317,6 +322,24 @@
     <t xml:space="preserve">Canteen OTH</t>
   </si>
   <si>
+    <t xml:space="preserve">PoS 2019 - IC HoReCa BarTavernClub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPIs_2019/PoS 2019 - IC HoReCa BarTavernClub.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PoS 2019 - IC HoReCa BarTavern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPIs_2019/Spirits 2018 - IC - HoReCa.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC - HoReCa All</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HoReCa</t>
+  </si>
+  <si>
     <t xml:space="preserve">PoS 2019 - IC HoReCa BarTavernClub - CAP</t>
   </si>
   <si>
@@ -326,15 +349,6 @@
     <t xml:space="preserve">PoS 2019 ICHoReCa BarTavern CAP</t>
   </si>
   <si>
-    <t xml:space="preserve">KPIs_2019/Spirits 2018 - IC - HoReCa.xlsx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IC - HoReCa All</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HoReCa</t>
-  </si>
-  <si>
     <t xml:space="preserve">PoS 2019 - IC HoReCa BarTavernClub - REG</t>
   </si>
   <si>
@@ -344,6 +358,12 @@
     <t xml:space="preserve">PoS 2019 ICHoReCa BarTavern REG</t>
   </si>
   <si>
+    <t xml:space="preserve">PoS 2019 - IC HoReCa RestCafeTea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPIs_2019/PoS 2019 - IC HoReCa RestCafeTea.xlsx</t>
+  </si>
+  <si>
     <t xml:space="preserve">PoS 2019 - IC HoReCa RestCafeTea - CAP</t>
   </si>
   <si>
@@ -386,10 +406,28 @@
     <t xml:space="preserve">KPIs_2019/PoS 2019 - IC QSR.xlsx</t>
   </si>
   <si>
-    <t xml:space="preserve">IC - QSR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QSR</t>
+    <t xml:space="preserve">IC - QSR-FastFood-Cinema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QSR-FastFood-Cinema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PoS 2019 - IC FastFood</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPIs_2019/PoS 2019 - IC FastFood.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PoS 2019 - IC Cinema - CAP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPIs_2019/PoS 2019 - IC Cinema - CAP.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PoS 2019 - IC Cinema - REG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPIs_2019/PoS 2019 - IC Cinema – REG.xlsx</t>
   </si>
   <si>
     <t xml:space="preserve">PoS 2019 - MT Conv Big - CAP</t>
@@ -719,10 +757,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.6683673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.265306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -877,10 +916,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.2091836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.6581632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.2091836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.6683673469388"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.25"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.6683673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1028,10 +1068,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.2091836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.6581632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.2091836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.6683673469388"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.25"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.6683673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1173,17 +1214,17 @@
   </sheetPr>
   <dimension ref="A1:D65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1316,11 +1357,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1453,11 +1494,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1590,11 +1631,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1727,11 +1768,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.2602040816326"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.8520408163265"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1887,11 +1928,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.2602040816326"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.8520408163265"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2042,16 +2083,16 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.530612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.2755102040816"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.1275510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="43.7397959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2203,21 +2244,22 @@
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="FF333333"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="P33" activeCellId="0" sqref="P33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.530612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.2755102040816"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.1275510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="43.7397959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2379,10 +2421,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.6683673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.265306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.3724489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2526,6 +2569,7 @@
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="FF333333"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D12"/>
@@ -2536,11 +2580,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.530612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.2755102040816"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.1275510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="43.7397959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2696,17 +2740,17 @@
   </sheetPr>
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.530612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.2755102040816"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.1275510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="43.7397959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2745,7 +2789,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2858,20 +2902,22 @@
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="FF333333"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.2091836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.6581632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.2091836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.1275510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="43.7397959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2893,10 +2939,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2909,8 +2955,8 @@
       <c r="C3" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>103</v>
+      <c r="D3" s="8" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2933,6 +2979,12 @@
       <c r="A6" s="0" t="s">
         <v>16</v>
       </c>
+      <c r="B6" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
@@ -2945,7 +2997,7 @@
         <v>80</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2959,7 +3011,7 @@
         <v>80</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2989,7 +3041,7 @@
         <v>65</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3017,20 +3069,22 @@
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="FF333333"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.2091836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.6581632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.2091836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.1275510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="43.7397959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3052,10 +3106,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3068,7 +3122,7 @@
       <c r="C3" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="8" t="s">
         <v>107</v>
       </c>
     </row>
@@ -3092,6 +3146,12 @@
       <c r="A6" s="0" t="s">
         <v>16</v>
       </c>
+      <c r="B6" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
@@ -3104,7 +3164,7 @@
         <v>80</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3118,7 +3178,7 @@
         <v>80</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3148,7 +3208,7 @@
         <v>65</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3186,10 +3246,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.2091836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.6581632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.2091836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.6683673469388"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.25"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.6683673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3211,10 +3272,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>109</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3228,7 +3289,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3263,7 +3324,7 @@
         <v>80</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3277,7 +3338,7 @@
         <v>80</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3307,7 +3368,7 @@
         <v>65</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3345,10 +3406,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.4234693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.6683673469388"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.25"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.6683673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3370,10 +3432,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>113</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3387,7 +3449,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3410,12 +3472,6 @@
       <c r="A6" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>115</v>
-      </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
@@ -3428,7 +3484,7 @@
         <v>80</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3442,7 +3498,7 @@
         <v>80</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3472,7 +3528,7 @@
         <v>65</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3505,15 +3561,16 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.4234693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.6683673469388"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.25"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.6683673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3535,10 +3592,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3552,7 +3609,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3575,12 +3632,6 @@
       <c r="A6" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>115</v>
-      </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
@@ -3596,7 +3647,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>22</v>
       </c>
@@ -3637,7 +3688,7 @@
         <v>65</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3670,15 +3721,16 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.3112244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.6683673469388"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.25"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.6683673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3700,10 +3752,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3717,7 +3769,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3740,12 +3792,6 @@
       <c r="A6" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>115</v>
-      </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
@@ -3761,7 +3807,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>22</v>
       </c>
@@ -3802,7 +3848,7 @@
         <v>65</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3834,16 +3880,17 @@
   </sheetPr>
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.3112244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.6683673469388"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.25"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.6683673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3865,10 +3912,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3882,7 +3929,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3905,12 +3952,6 @@
       <c r="A6" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>115</v>
-      </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
@@ -3926,7 +3967,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>22</v>
       </c>
@@ -3967,7 +4008,7 @@
         <v>65</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4000,15 +4041,16 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.6683673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.6683673469388"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.25"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.6683673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4030,13 +4072,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>7</v>
       </c>
@@ -4047,7 +4089,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4070,12 +4112,6 @@
       <c r="A6" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>127</v>
-      </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
@@ -4088,10 +4124,10 @@
         <v>80</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>22</v>
       </c>
@@ -4102,7 +4138,7 @@
         <v>80</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4132,7 +4168,7 @@
         <v>65</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4170,10 +4206,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.6683673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.265306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.3724489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4327,10 +4364,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.6683673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.0204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.3724489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4352,10 +4390,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4369,7 +4407,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4393,10 +4431,10 @@
         <v>16</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4410,7 +4448,7 @@
         <v>80</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4424,7 +4462,7 @@
         <v>80</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4454,7 +4492,7 @@
         <v>65</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4492,10 +4530,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.3928571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.0204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.3724489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4517,10 +4556,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4534,7 +4573,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4558,10 +4597,10 @@
         <v>16</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4575,7 +4614,7 @@
         <v>80</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4589,7 +4628,7 @@
         <v>80</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4619,7 +4658,7 @@
         <v>65</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4657,10 +4696,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.7959183673469"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.7704081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.3724489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4682,10 +4722,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4699,7 +4739,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4723,10 +4763,10 @@
         <v>16</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4740,7 +4780,7 @@
         <v>80</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4754,7 +4794,7 @@
         <v>80</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4784,7 +4824,837 @@
         <v>65</v>
       </c>
       <c r="D11" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.7704081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.3724489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.265306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.3724489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>138</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.265306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.3724489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.9897959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.3724489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.3928571428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.3724489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4822,10 +5692,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.6683673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.265306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.3724489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4979,10 +5850,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.6683673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.265306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.3724489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5136,10 +6008,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.2091836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.6581632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.2091836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.6683673469388"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.25"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.6683673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5293,10 +6166,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.2091836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.6581632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.2091836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.6683673469388"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.25"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.6683673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5450,10 +6324,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.2091836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.6581632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.2091836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.6683673469388"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.25"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.6683673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5607,10 +6482,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.2091836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.6581632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.2091836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.6683673469388"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.25"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.6683673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
PROS-13075 - CCRU - POS 2020 KPIs
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/KPI_Source.xlsx
+++ b/Projects/CCRU/Data/KPI_Source.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="POS" sheetId="1" state="visible" r:id="rId2"/>
@@ -599,7 +599,7 @@
     <t xml:space="preserve">FT S</t>
   </si>
   <si>
-    <t xml:space="preserve">Conv BIG CAP-NKA</t>
+    <t xml:space="preserve">Conv Big CAP-NKA</t>
   </si>
   <si>
     <t xml:space="preserve">Conv Small</t>
@@ -608,7 +608,7 @@
     <t xml:space="preserve">Super</t>
   </si>
   <si>
-    <t xml:space="preserve">Conv BIG REG</t>
+    <t xml:space="preserve">Conv Big REG</t>
   </si>
   <si>
     <t xml:space="preserve">IC BarNight-CoffeeShop</t>
@@ -937,7 +937,7 @@
   </sheetPr>
   <dimension ref="A1:F78"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="C36" activeCellId="0" sqref="C36"/>
@@ -945,13 +945,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.0769230769231"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.5627530364373"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="58.7287449392713"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.7651821862348"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.4251012145749"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.7651821862348"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.1983805668016"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.8178137651822"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.5303643724696"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="67.9838056680162"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.7368421052632"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="22.3967611336032"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.7368421052632"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.1417004048583"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2428,12 +2428,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.0769230769231"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.5627530364373"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="58.7287449392713"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.7651821862348"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.4251012145749"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.1983805668016"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.8178137651822"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.5303643724696"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="67.9838056680162"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.7368421052632"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="22.3967611336032"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.1417004048583"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3020,12 +3020,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.0769230769231"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.5627530364373"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="58.7287449392713"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.7651821862348"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.4251012145749"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.1983805668016"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.8178137651822"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.5303643724696"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="67.9838056680162"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.7368421052632"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="22.3967611336032"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.1417004048583"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3560,12 +3560,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.0769230769231"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.5627530364373"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="58.7287449392713"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.7651821862348"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.4251012145749"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.1983805668016"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.8178137651822"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.5303643724696"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="67.9838056680162"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.7368421052632"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="22.3967611336032"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.1417004048583"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4248,20 +4248,20 @@
   </sheetPr>
   <dimension ref="A1:E78"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B39" activeCellId="0" sqref="B39"/>
+      <selection pane="bottomLeft" activeCell="C58" activeCellId="0" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.0769230769231"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.5627530364373"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="58.7287449392713"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.7651821862348"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.4251012145749"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.1983805668016"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.8178137651822"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.5303643724696"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="67.9838056680162"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.7368421052632"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="22.3967611336032"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.1417004048583"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5312,12 +5312,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.0769230769231"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.5627530364373"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="58.7287449392713"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.7651821862348"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.4251012145749"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.1983805668016"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.8178137651822"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.5303643724696"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="67.9838056680162"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.7368421052632"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="22.3967611336032"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.1417004048583"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6246,12 +6246,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.0769230769231"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.5627530364373"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="58.7287449392713"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.7651821862348"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.4251012145749"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.1983805668016"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.8178137651822"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.5303643724696"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="67.9838056680162"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.7368421052632"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="22.3967611336032"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.1417004048583"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7180,12 +7180,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.0769230769231"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.5627530364373"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="58.7287449392713"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.7651821862348"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.4251012145749"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.1983805668016"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.8178137651822"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.5303643724696"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="67.9838056680162"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.7368421052632"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="22.3967611336032"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.1417004048583"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7992,12 +7992,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.0769230769231"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.5627530364373"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="58.7287449392713"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.7651821862348"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.4251012145749"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.1983805668016"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.8178137651822"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.5303643724696"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="67.9838056680162"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.7368421052632"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="22.3967611336032"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.1417004048583"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8803,12 +8803,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.0769230769231"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.5627530364373"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="58.7287449392713"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.7651821862348"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.4251012145749"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.1983805668016"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.8178137651822"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.5303643724696"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="67.9838056680162"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.7368421052632"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="22.3967611336032"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.1417004048583"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9861,12 +9861,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.0769230769231"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.5627530364373"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="58.7287449392713"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.7651821862348"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.4251012145749"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.1983805668016"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.8178137651822"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.5303643724696"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="67.9838056680162"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.7368421052632"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="22.3967611336032"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.1417004048583"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>